<commit_message>
Leitungsparameter koennen auch als 0 eingelesen werden.
</commit_message>
<xml_diff>
--- a/test/test_files/LineParameters.xlsx
+++ b/test/test_files/LineParameters.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2F2BF2-82B3-4DE3-A188-D83589E2B062}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequenz enthalten" sheetId="1" r:id="rId1"/>
     <sheet name="ohne Frequenz" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Knoten 2</t>
   </si>
@@ -62,7 +69,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">x_quer in </t>
+      <t xml:space="preserve">x_len in </t>
     </r>
     <r>
       <rPr>
@@ -76,8 +83,38 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">x_len in </t>
+    <t>Quelle:</t>
+  </si>
+  <si>
+    <t>https://ub-deposit.fernuni-hagen.de/servlets/MCRFileNodeServlet/mir_derivate_00000097/Diss_Wille-Haussmann_Smart_Grid_2011.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabeltyp: </t>
+  </si>
+  <si>
+    <t>NYY 4x50</t>
+  </si>
+  <si>
+    <t>Seite in PDF:</t>
+  </si>
+  <si>
+    <r>
+      <t>L' in mH</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>/km</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">R' in </t>
     </r>
     <r>
       <rPr>
@@ -91,23 +128,8 @@
     </r>
   </si>
   <si>
-    <t>Quelle:</t>
-  </si>
-  <si>
-    <t>https://ub-deposit.fernuni-hagen.de/servlets/MCRFileNodeServlet/mir_derivate_00000097/Diss_Wille-Haussmann_Smart_Grid_2011.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kabeltyp: </t>
-  </si>
-  <si>
-    <t>NYY 4x50</t>
-  </si>
-  <si>
-    <t>Seite in PDF:</t>
-  </si>
-  <si>
-    <r>
-      <t>L' in mH</t>
+    <r>
+      <t>C' in nF</t>
     </r>
     <r>
       <rPr>
@@ -121,8 +143,23 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">R' in </t>
+    <t>Frequenz in Hz:</t>
+  </si>
+  <si>
+    <t>x_quer in Ω/km</t>
+  </si>
+  <si>
+    <t>Netztyp</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Stadt, Gewerbe</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">g_quer in </t>
     </r>
     <r>
       <rPr>
@@ -137,7 +174,7 @@
   </si>
   <si>
     <r>
-      <t>C' in nF</t>
+      <t xml:space="preserve">b_quer in </t>
     </r>
     <r>
       <rPr>
@@ -147,20 +184,14 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>/km</t>
-    </r>
-  </si>
-  <si>
-    <t>Frequenz in Hz:</t>
-  </si>
-  <si>
-    <t>x_quer in Ω/km</t>
+      <t>Ω/km</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -499,199 +530,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.437</v>
+      </c>
+      <c r="B2">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="D2" s="2">
+        <v>1.02E-8</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.157</v>
+      </c>
+      <c r="B3">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0.437</v>
-      </c>
-      <c r="D2">
-        <v>0.30199999999999999</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1.02E-8</v>
-      </c>
-      <c r="G2">
-        <v>0.2</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>0.437</v>
-      </c>
-      <c r="D3">
-        <v>0.30199999999999999</v>
+      <c r="D3" s="2">
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
-        <v>1.02E-8</v>
-      </c>
-      <c r="G3">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>0.437</v>
-      </c>
-      <c r="D4">
-        <v>0.30199999999999999</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.02E-8</v>
-      </c>
-      <c r="G4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>0.437</v>
-      </c>
-      <c r="D5">
-        <v>0.30199999999999999</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.02E-8</v>
-      </c>
-      <c r="G5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>0.437</v>
-      </c>
-      <c r="D6">
-        <v>0.30199999999999999</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.02E-8</v>
-      </c>
-      <c r="G6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>0.437</v>
-      </c>
-      <c r="D7">
-        <v>0.30199999999999999</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.02E-8</v>
-      </c>
-      <c r="G7">
-        <v>0.5</v>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J1" r:id="rId1"/>
+    <hyperlink ref="I1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -699,7 +630,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -723,31 +654,31 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -781,7 +712,7 @@
         <v>0.2</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L2">
         <v>50</v>
@@ -818,10 +749,10 @@
         <v>0.3</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -855,7 +786,7 @@
         <v>0.4</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L4">
         <v>37</v>
@@ -956,7 +887,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L3" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>